<commit_message>
folder files creation new
</commit_message>
<xml_diff>
--- a/bin/com/cpb/testdata/testdata.xlsx
+++ b/bin/com/cpb/testdata/testdata.xlsx
@@ -3,17 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A4970AD7-5F23-485B-B1A6-04291D92828D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9956A236-4D45-43C5-899B-192FFE133AC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="17235" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="17535" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M24"/>
+  <oleSize ref="A1:L13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,34 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>A234wd</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>TCID</t>
   </si>
@@ -58,21 +30,9 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>runmode</t>
   </si>
   <si>
@@ -82,22 +42,16 @@
     <t>cd</t>
   </si>
   <si>
-    <t>efgh</t>
-  </si>
-  <si>
-    <t>ij</t>
-  </si>
-  <si>
-    <t>kl</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>cs</t>
-  </si>
-  <si>
-    <t>ab cd</t>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>RowId</t>
   </si>
 </sst>
 </file>
@@ -417,175 +371,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>